<commit_message>
added new dashboard design
</commit_message>
<xml_diff>
--- a/public/outputs/abonnements.xlsx
+++ b/public/outputs/abonnements.xlsx
@@ -42,9 +42,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -376,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -389,33 +388,9 @@
         <v>E-Mail</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="1">
-        <v>44378.99939740741</v>
-      </c>
-      <c r="B2" t="str">
-        <v>johnvhardenberg@googlemail.com</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1">
-        <v>44379.99625038195</v>
-      </c>
-      <c r="B3" t="str">
-        <v>john.hardenberg123@gmail.com</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1">
-        <v>44380.01841818287</v>
-      </c>
-      <c r="B4" t="str">
-        <v>johnprogrammieren@gmail.com</v>
-      </c>
-    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:B4"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:B1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>